<commit_message>
Work plan, documentation and read me updated
</commit_message>
<xml_diff>
--- a/Documentation/Work Plan.xlsx
+++ b/Documentation/Work Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed Sayed Mansour\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Education\Git\Text-Classification-GP\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Task Name</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>Start Meeting to fing idea</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>Testing our models</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Testing our Back end</t>
   </si>
   <si>
@@ -167,29 +161,56 @@
     <t>20/5/2021</t>
   </si>
   <si>
-    <t>25/5/2021</t>
-  </si>
-  <si>
-    <t>23/5/2021</t>
-  </si>
-  <si>
     <t>21/5/2021</t>
   </si>
   <si>
     <t>18/5/2021</t>
   </si>
   <si>
-    <t>20/1/2021</t>
-  </si>
-  <si>
-    <t>24/5/2021</t>
+    <t>Adding all big size models to our web application</t>
+  </si>
+  <si>
+    <t>Training on big data(arxiv dataset)</t>
+  </si>
+  <si>
+    <t>Comparing models to choose the best for arxiv</t>
+  </si>
+  <si>
+    <t>22/5/2021</t>
+  </si>
+  <si>
+    <t>30/5/2021</t>
+  </si>
+  <si>
+    <t>cleaning the arxiv dataset</t>
+  </si>
+  <si>
+    <t>13/7/2021</t>
+  </si>
+  <si>
+    <t>15/7/2021</t>
+  </si>
+  <si>
+    <t>Updating all diagrams with new updates</t>
+  </si>
+  <si>
+    <t>16/7/2021</t>
+  </si>
+  <si>
+    <t>20/7/2021</t>
+  </si>
+  <si>
+    <t>22/7/2021</t>
+  </si>
+  <si>
+    <t>Start Meeting to find idea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +220,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -231,23 +259,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -262,7 +295,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -277,7 +310,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -290,7 +323,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -303,7 +336,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -316,7 +349,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -324,6 +357,7 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -340,6 +374,7 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -355,8 +390,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D30"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Task Name" dataDxfId="3"/>
     <tableColumn id="2" name="Status" dataDxfId="2"/>
@@ -630,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,7 +679,7 @@
     <col min="4" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -658,341 +693,403 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7">
+        <v>43840</v>
+      </c>
+      <c r="D8" s="7">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>43900</v>
+      </c>
+      <c r="D9" s="8">
+        <v>43931</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8">
+        <v>43931</v>
+      </c>
+      <c r="D10" s="8">
+        <v>43992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>43992</v>
+      </c>
+      <c r="D11" s="8">
+        <v>44114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8">
+        <v>44114</v>
+      </c>
+      <c r="D12" s="8">
+        <v>44175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8">
+        <v>44175</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="7">
+        <v>44201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="6">
-        <v>43840</v>
-      </c>
-      <c r="D8" s="6">
-        <v>43900</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7">
-        <v>43900</v>
-      </c>
-      <c r="D9" s="7">
-        <v>43931</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="7">
-        <v>43931</v>
-      </c>
-      <c r="D10" s="7">
-        <v>43992</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7">
-        <v>43992</v>
-      </c>
-      <c r="D11" s="7">
-        <v>44114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="7">
-        <v>44114</v>
-      </c>
-      <c r="D12" s="7">
-        <v>44175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="D18" s="7">
+        <v>44321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7">
+        <v>43841</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="7">
+        <v>43962</v>
+      </c>
+      <c r="D20" s="7">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7">
+        <v>44200</v>
+      </c>
+      <c r="D21" s="7">
+        <v>44320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="7">
+        <v>44197</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="7">
+        <v>44287</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7">
+        <v>44384</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="7">
-        <v>44175</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="6">
-        <v>44201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="6">
-        <v>44321</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="6">
-        <v>43841</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="6">
-        <v>43962</v>
-      </c>
-      <c r="D20" s="6">
-        <v>44444</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="6">
-        <v>44200</v>
-      </c>
-      <c r="D21" s="6">
-        <v>44320</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="6">
-        <v>44197</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="6">
-        <v>44287</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="B30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>